<commit_message>
Atualizado IM em geral.
</commit_message>
<xml_diff>
--- a/outputs/sisaprophelper#autoaprop/autoapropxlsx/IMC.XLSX
+++ b/outputs/sisaprophelper#autoaprop/autoapropxlsx/IMC.XLSX
@@ -150,6 +150,9 @@
     <t>IQ-DOC</t>
   </si>
   <si>
+    <t>KENI CAETANO ANTUNES MALAQUIAS</t>
+  </si>
+  <si>
     <t>ALEXANDRE FRAGA VIANA</t>
   </si>
   <si>
@@ -159,9 +162,21 @@
     <t>AMARILDO ROSA PEREIRA</t>
   </si>
   <si>
+    <t>VANIA MARQUES DA COSTA</t>
+  </si>
+  <si>
+    <t>DAVI DOS SANTOS NEVES</t>
+  </si>
+  <si>
+    <t>MARCELO TORRES DE QUEIROZ</t>
+  </si>
+  <si>
     <t>ANTONIO CARLOS DE O FLEURY</t>
   </si>
   <si>
+    <t>JULIANA DE OLIVEIRA DOS SANTOS</t>
+  </si>
+  <si>
     <t>RICARDO KENJI MATSUO</t>
   </si>
   <si>
@@ -225,19 +240,7 @@
     <t> </t>
   </si>
   <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
+    <t>1098</t>
   </si>
   <si>
     <t>2572</t>
@@ -249,28 +252,25 @@
     <t>2727</t>
   </si>
   <si>
+    <t>2932</t>
+  </si>
+  <si>
+    <t>3120</t>
+  </si>
+  <si>
+    <t>3152</t>
+  </si>
+  <si>
     <t>3501</t>
   </si>
   <si>
+    <t>3519</t>
+  </si>
+  <si>
     <t>3961</t>
   </si>
   <si>
     <t>3963</t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
-  </si>
-  <si>
-    <t> </t>
   </si>
   <si>
     <t> </t>

</xml_diff>